<commit_message>
Fixed bug where classes were being unaccounted for because of my silly way of delimitting. Fixed bug where stat would not show up because STAT would show up in another School and I wasn't resetting the course. Updated all the db files because of the error of classes being unaccounted for.
</commit_message>
<xml_diff>
--- a/GradeDistributionsDB/Fall2013/Output/Fall2013 EL.xlsx
+++ b/GradeDistributionsDB/Fall2013/Output/Fall2013 EL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
   <si>
     <t>Course</t>
   </si>
@@ -145,6 +145,21 @@
     <t>3.23%</t>
   </si>
   <si>
+    <t>FLACY K</t>
+  </si>
+  <si>
+    <t>22.22%</t>
+  </si>
+  <si>
+    <t>61.11%</t>
+  </si>
+  <si>
+    <t>11.11%</t>
+  </si>
+  <si>
+    <t>5.56%</t>
+  </si>
+  <si>
     <t>DOWNEY M</t>
   </si>
   <si>
@@ -166,15 +181,9 @@
     <t>44.44%</t>
   </si>
   <si>
-    <t>22.22%</t>
-  </si>
-  <si>
     <t>66.67%</t>
   </si>
   <si>
-    <t>11.11%</t>
-  </si>
-  <si>
     <t>ELIE-100</t>
   </si>
   <si>
@@ -209,9 +218,6 @@
   </si>
   <si>
     <t>ELIG-250</t>
-  </si>
-  <si>
-    <t>FLACY K</t>
   </si>
   <si>
     <t>30.00%</t>
@@ -755,7 +761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -998,551 +1004,551 @@
         <v>43</v>
       </c>
       <c r="C17" t="n">
+        <v>2.944</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="n">
         <v>2.2375</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>41</v>
       </c>
-      <c r="F17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" t="s">
         <v>39</v>
       </c>
-      <c r="H17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>46</v>
+      <c r="H18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
+      <c r="A20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C21" t="n">
-        <v>2.778</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
         <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="n">
+        <v>2.778</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C23" t="n">
         <v>3</v>
       </c>
-      <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>52</v>
       </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="n">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="n">
+      <c r="C29" t="n">
         <v>2.579</v>
       </c>
-      <c r="D28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2.6165</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2.678</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2.923</v>
+      </c>
+      <c r="D41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2.531</v>
+      </c>
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" t="s">
+        <v>87</v>
+      </c>
+      <c r="H47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" t="n">
+        <v>2.3585</v>
+      </c>
+      <c r="D50" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="B53" t="s">
         <v>57</v>
       </c>
-      <c r="F28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" t="s">
-        <v>59</v>
-      </c>
-      <c r="H28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="n">
-        <v>2.6165</v>
-      </c>
-      <c r="D31" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F34" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" t="s">
-        <v>36</v>
-      </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="B37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" t="n">
-        <v>2.678</v>
-      </c>
-      <c r="D37" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" t="s">
-        <v>70</v>
-      </c>
-      <c r="G37" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" t="n">
-        <v>2.923</v>
-      </c>
-      <c r="D40" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="C53" t="n">
+        <v>2.571</v>
+      </c>
+      <c r="D53" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" t="s">
         <v>11</v>
       </c>
-      <c r="F40" t="s">
-        <v>77</v>
-      </c>
-      <c r="G40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="B43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" t="n">
-        <v>2.531</v>
-      </c>
-      <c r="D43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" t="s">
         <v>11</v>
       </c>
-      <c r="F43" t="s">
-        <v>78</v>
-      </c>
-      <c r="G43" t="s">
-        <v>77</v>
-      </c>
-      <c r="H43" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="B46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" t="n">
-        <v>2.375</v>
-      </c>
-      <c r="D46" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46" t="s">
-        <v>84</v>
-      </c>
-      <c r="F46" t="s">
-        <v>85</v>
-      </c>
-      <c r="G46" t="s">
-        <v>85</v>
-      </c>
-      <c r="H46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" t="n">
-        <v>2.3585</v>
-      </c>
-      <c r="D49" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" t="s">
-        <v>63</v>
-      </c>
-      <c r="G49" t="s">
-        <v>58</v>
-      </c>
-      <c r="H49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="B52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" t="n">
-        <v>2.571</v>
-      </c>
-      <c r="D52" t="s">
-        <v>76</v>
-      </c>
-      <c r="E52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" t="s">
-        <v>15</v>
-      </c>
-      <c r="G52" t="s">
-        <v>15</v>
-      </c>
-      <c r="H52" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="B55" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" t="n">
-        <v>2.7565</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="A55" t="s">
         <v>93</v>
-      </c>
-      <c r="E55" t="s">
-        <v>94</v>
-      </c>
-      <c r="F55" t="s">
-        <v>36</v>
-      </c>
-      <c r="G55" t="s">
-        <v>95</v>
-      </c>
-      <c r="H55" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="B56" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C56" t="n">
-        <v>2.5</v>
+        <v>2.7565</v>
       </c>
       <c r="D56" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="E56" t="s">
         <v>96</v>
       </c>
       <c r="F56" t="s">
+        <v>36</v>
+      </c>
+      <c r="G56" t="s">
         <v>97</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" t="s">
+        <v>99</v>
+      </c>
+      <c r="G57" t="s">
         <v>10</v>
       </c>
-      <c r="H56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" t="s">
-        <v>98</v>
+      <c r="H57" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="B59" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" t="n">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" t="s">
-        <v>49</v>
-      </c>
-      <c r="F59" t="s">
-        <v>52</v>
-      </c>
-      <c r="G59" t="s">
-        <v>15</v>
-      </c>
-      <c r="H59" t="s">
-        <v>99</v>
+      <c r="A59" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="B60" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C60" t="n">
-        <v>1.546</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E60" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="F60" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G60" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H60" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" t="s">
+    <row r="61" spans="1:8">
+      <c r="B61" t="s">
         <v>102</v>
       </c>
+      <c r="C61" t="n">
+        <v>1.546</v>
+      </c>
+      <c r="D61" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="B63" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" t="n">
+      <c r="A63" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="n">
         <v>2.714</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>12</v>
       </c>
-      <c r="E63" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E64" t="s">
+        <v>98</v>
+      </c>
+      <c r="F64" t="s">
         <v>12</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G64" t="s">
         <v>12</v>
       </c>
-      <c r="H63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" t="s">
-        <v>103</v>
+      <c r="H64" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" t="n">
-        <v>2.273</v>
-      </c>
-      <c r="D66" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" t="s">
-        <v>101</v>
-      </c>
-      <c r="F66" t="s">
-        <v>17</v>
-      </c>
-      <c r="G66" t="s">
-        <v>15</v>
-      </c>
-      <c r="H66" t="s">
-        <v>104</v>
+      <c r="A66" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="B67" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C67" t="n">
-        <v>2.636</v>
+        <v>2.273</v>
       </c>
       <c r="D67" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="E67" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F67" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="G67" t="s">
         <v>15</v>
@@ -1553,341 +1559,364 @@
     </row>
     <row r="68" spans="1:8">
       <c r="B68" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="C68" t="n">
+        <v>2.636</v>
+      </c>
+      <c r="D68" t="s">
+        <v>107</v>
+      </c>
+      <c r="E68" t="s">
+        <v>103</v>
+      </c>
+      <c r="F68" t="s">
+        <v>106</v>
+      </c>
+      <c r="G68" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" t="n">
         <v>2.909</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>18</v>
       </c>
-      <c r="E68" t="s">
-        <v>107</v>
-      </c>
-      <c r="F68" t="s">
-        <v>104</v>
-      </c>
-      <c r="G68" t="s">
-        <v>15</v>
-      </c>
-      <c r="H68" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" t="s">
-        <v>108</v>
+      <c r="E69" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69" t="s">
+        <v>106</v>
+      </c>
+      <c r="G69" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="B71" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" t="n">
+      <c r="A71" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="B72" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" t="n">
         <v>2.678</v>
       </c>
-      <c r="D71" t="s">
-        <v>109</v>
-      </c>
-      <c r="E71" t="s">
-        <v>110</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="D72" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72" t="s">
+        <v>112</v>
+      </c>
+      <c r="F72" t="s">
         <v>36</v>
       </c>
-      <c r="G71" t="s">
-        <v>111</v>
-      </c>
-      <c r="H71" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" t="s">
+      <c r="G72" t="s">
         <v>113</v>
       </c>
+      <c r="H72" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="B74" t="s">
-        <v>100</v>
-      </c>
-      <c r="C74" t="n">
-        <v>2</v>
-      </c>
-      <c r="D74" t="s">
-        <v>37</v>
-      </c>
-      <c r="E74" t="s">
-        <v>66</v>
-      </c>
-      <c r="F74" t="s">
-        <v>66</v>
-      </c>
-      <c r="G74" t="s">
-        <v>37</v>
-      </c>
-      <c r="H74" t="s">
-        <v>36</v>
+      <c r="A74" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="B75" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C75" t="n">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>37</v>
+      </c>
+      <c r="E75" t="s">
+        <v>68</v>
+      </c>
+      <c r="F75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G75" t="s">
+        <v>37</v>
+      </c>
+      <c r="H75" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="B76" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" t="n">
         <v>2.6675</v>
       </c>
-      <c r="D75" t="s">
-        <v>50</v>
-      </c>
-      <c r="E75" t="s">
-        <v>49</v>
-      </c>
-      <c r="F75" t="s">
-        <v>114</v>
-      </c>
-      <c r="G75" t="s">
-        <v>115</v>
-      </c>
-      <c r="H75" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="A77" t="s">
+      <c r="D76" t="s">
+        <v>44</v>
+      </c>
+      <c r="E76" t="s">
+        <v>54</v>
+      </c>
+      <c r="F76" t="s">
         <v>116</v>
       </c>
+      <c r="G76" t="s">
+        <v>117</v>
+      </c>
+      <c r="H76" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="78" spans="1:8">
-      <c r="B78" t="s">
-        <v>69</v>
-      </c>
-      <c r="C78" t="n">
+      <c r="A78" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="B79" t="s">
+        <v>71</v>
+      </c>
+      <c r="C79" t="n">
         <v>2.333</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" t="s">
         <v>33</v>
       </c>
-      <c r="E78" t="s">
-        <v>49</v>
-      </c>
-      <c r="F78" t="s">
-        <v>52</v>
-      </c>
-      <c r="G78" t="s">
-        <v>52</v>
-      </c>
-      <c r="H78" t="s">
+      <c r="E79" t="s">
+        <v>54</v>
+      </c>
+      <c r="F79" t="s">
+        <v>46</v>
+      </c>
+      <c r="G79" t="s">
+        <v>46</v>
+      </c>
+      <c r="H79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="81" spans="1:8">
-      <c r="B81" t="s">
-        <v>88</v>
-      </c>
-      <c r="C81" t="n">
-        <v>2.176</v>
-      </c>
-      <c r="D81" t="s">
-        <v>118</v>
-      </c>
-      <c r="E81" t="s">
+      <c r="A81" t="s">
         <v>119</v>
-      </c>
-      <c r="F81" t="s">
-        <v>118</v>
-      </c>
-      <c r="G81" t="s">
-        <v>120</v>
-      </c>
-      <c r="H81" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="B82" t="s">
+        <v>90</v>
+      </c>
+      <c r="C82" t="n">
+        <v>2.176</v>
+      </c>
+      <c r="D82" t="s">
+        <v>120</v>
+      </c>
+      <c r="E82" t="s">
+        <v>121</v>
+      </c>
+      <c r="F82" t="s">
+        <v>120</v>
+      </c>
+      <c r="G82" t="s">
+        <v>122</v>
+      </c>
+      <c r="H82" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="B83" t="s">
         <v>24</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C83" t="n">
         <v>1.938</v>
       </c>
-      <c r="D82" t="s">
-        <v>15</v>
-      </c>
-      <c r="E82" t="s">
-        <v>84</v>
-      </c>
-      <c r="F82" t="s">
-        <v>83</v>
-      </c>
-      <c r="G82" t="s">
-        <v>15</v>
-      </c>
-      <c r="H82" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" t="s">
-        <v>123</v>
+      <c r="D83" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" t="s">
+        <v>86</v>
+      </c>
+      <c r="F83" t="s">
+        <v>85</v>
+      </c>
+      <c r="G83" t="s">
+        <v>15</v>
+      </c>
+      <c r="H83" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="B85" t="s">
+      <c r="A85" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="B86" t="s">
         <v>14</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C86" t="n">
         <v>2.9885</v>
       </c>
-      <c r="D85" t="s">
-        <v>124</v>
-      </c>
-      <c r="E85" t="s">
-        <v>125</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="D86" t="s">
+        <v>126</v>
+      </c>
+      <c r="E86" t="s">
+        <v>127</v>
+      </c>
+      <c r="F86" t="s">
         <v>18</v>
       </c>
-      <c r="G85" t="s">
-        <v>70</v>
-      </c>
-      <c r="H85" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" t="s">
-        <v>126</v>
+      <c r="G86" t="s">
+        <v>72</v>
+      </c>
+      <c r="H86" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="B88" t="s">
-        <v>65</v>
-      </c>
-      <c r="C88" t="n">
-        <v>2.214</v>
-      </c>
-      <c r="D88" t="s">
-        <v>13</v>
-      </c>
-      <c r="E88" t="s">
-        <v>12</v>
-      </c>
-      <c r="F88" t="s">
-        <v>76</v>
-      </c>
-      <c r="G88" t="s">
-        <v>10</v>
-      </c>
-      <c r="H88" t="s">
-        <v>12</v>
+      <c r="A88" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="B89" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C89" t="n">
+        <v>2.214</v>
+      </c>
+      <c r="D89" t="s">
+        <v>13</v>
+      </c>
+      <c r="E89" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" t="s">
+        <v>78</v>
+      </c>
+      <c r="G89" t="s">
+        <v>10</v>
+      </c>
+      <c r="H89" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="B90" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" t="n">
         <v>1.546</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
         <v>18</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E90" t="s">
         <v>16</v>
       </c>
-      <c r="F89" t="s">
-        <v>15</v>
-      </c>
-      <c r="G89" t="s">
+      <c r="F90" t="s">
+        <v>15</v>
+      </c>
+      <c r="G90" t="s">
         <v>18</v>
       </c>
-      <c r="H89" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" t="s">
-        <v>127</v>
+      <c r="H90" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:8">
-      <c r="B92" t="s">
+      <c r="A92" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="B93" t="s">
         <v>30</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C93" t="n">
         <v>2.684</v>
       </c>
-      <c r="D92" t="s">
-        <v>128</v>
-      </c>
-      <c r="E92" t="s">
-        <v>129</v>
-      </c>
-      <c r="F92" t="s">
-        <v>59</v>
-      </c>
-      <c r="G92" t="s">
-        <v>60</v>
-      </c>
-      <c r="H92" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" t="s">
+      <c r="D93" t="s">
         <v>130</v>
       </c>
+      <c r="E93" t="s">
+        <v>131</v>
+      </c>
+      <c r="F93" t="s">
+        <v>62</v>
+      </c>
+      <c r="G93" t="s">
+        <v>63</v>
+      </c>
+      <c r="H93" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="95" spans="1:8">
-      <c r="B95" t="s">
-        <v>24</v>
-      </c>
-      <c r="C95" t="n">
-        <v>2.933</v>
-      </c>
-      <c r="D95" t="s">
-        <v>67</v>
-      </c>
-      <c r="E95" t="s">
-        <v>99</v>
-      </c>
-      <c r="F95" t="s">
-        <v>131</v>
-      </c>
-      <c r="G95" t="s">
-        <v>132</v>
-      </c>
-      <c r="H95" t="s">
+      <c r="A95" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="96" spans="1:8">
       <c r="B96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" t="n">
+        <v>2.933</v>
+      </c>
+      <c r="D96" t="s">
+        <v>69</v>
+      </c>
+      <c r="E96" t="s">
+        <v>101</v>
+      </c>
+      <c r="F96" t="s">
+        <v>133</v>
+      </c>
+      <c r="G96" t="s">
+        <v>134</v>
+      </c>
+      <c r="H96" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="B97" t="s">
         <v>34</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C97" t="n">
         <v>2.79</v>
       </c>
-      <c r="D96" t="s">
-        <v>133</v>
-      </c>
-      <c r="E96" t="s">
-        <v>134</v>
-      </c>
-      <c r="F96" t="s">
-        <v>60</v>
-      </c>
-      <c r="G96" t="s">
-        <v>58</v>
-      </c>
-      <c r="H96" t="s">
-        <v>59</v>
+      <c r="D97" t="s">
+        <v>135</v>
+      </c>
+      <c r="E97" t="s">
+        <v>136</v>
+      </c>
+      <c r="F97" t="s">
+        <v>63</v>
+      </c>
+      <c r="G97" t="s">
+        <v>61</v>
+      </c>
+      <c r="H97" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add q drop to master db
</commit_message>
<xml_diff>
--- a/GradeDistributionsDB/Fall2013/Output/Fall2013 EL.xlsx
+++ b/GradeDistributionsDB/Fall2013/Output/Fall2013 EL.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
   <si>
     <t>Course</t>
   </si>
@@ -40,6 +40,9 @@
     <t>% of F's</t>
   </si>
   <si>
+    <t>% of Q Drop's</t>
+  </si>
+  <si>
     <t>ELIC-100</t>
   </si>
   <si>
@@ -58,10 +61,10 @@
     <t>21.43%</t>
   </si>
   <si>
+    <t>0.00%</t>
+  </si>
+  <si>
     <t>DAVIS S</t>
-  </si>
-  <si>
-    <t>0.00%</t>
   </si>
   <si>
     <t>36.36%</t>
@@ -462,12 +465,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -761,15 +763,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -794,38 +796,44 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
         <v>1.643</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
         <v>1.909</v>
@@ -834,49 +842,55 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="n">
         <v>2.615</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="n">
         <v>2.917</v>
@@ -885,10 +899,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -896,61 +910,70 @@
       <c r="H8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
         <v>2.615</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="B12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" t="n">
         <v>2.5</v>
@@ -959,106 +982,118 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" t="n">
         <v>2.5145</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" t="n">
         <v>2.944</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>48</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" t="n">
         <v>2.2375</v>
       </c>
       <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
         <v>42</v>
       </c>
-      <c r="E18" t="s">
-        <v>41</v>
-      </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>51</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="B21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C21" t="n">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -1072,42 +1107,48 @@
       <c r="H21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="B22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" t="n">
         <v>2.778</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G22" t="s">
         <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>34</v>
+      </c>
+      <c r="I22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="B23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" t="n">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -1116,23 +1157,26 @@
         <v>15</v>
       </c>
       <c r="H23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>45</v>
+      </c>
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="B26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" t="n">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -1146,248 +1190,275 @@
       <c r="H26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="B29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C29" t="n">
         <v>2.579</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>64</v>
+      </c>
+      <c r="I29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32" t="n">
         <v>2.6165</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>63</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="B35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C35" t="n">
         <v>2.3</v>
       </c>
       <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" t="s">
         <v>37</v>
       </c>
-      <c r="E35" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" t="s">
-        <v>36</v>
-      </c>
       <c r="H35" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="B38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C38" t="n">
         <v>2.678</v>
       </c>
       <c r="D38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E38" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" t="s">
         <v>73</v>
       </c>
-      <c r="F38" t="s">
-        <v>72</v>
-      </c>
       <c r="G38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>76</v>
+      </c>
+      <c r="I38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="B41" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C41" t="n">
         <v>2.923</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G41" t="s">
         <v>15</v>
       </c>
       <c r="H41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>81</v>
+      </c>
+      <c r="I41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="B44" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C44" t="n">
         <v>2.531</v>
       </c>
       <c r="D44" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" t="s">
         <v>80</v>
       </c>
-      <c r="G44" t="s">
-        <v>79</v>
-      </c>
       <c r="H44" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>81</v>
+      </c>
+      <c r="I44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="B47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C47" t="n">
         <v>2.375</v>
       </c>
       <c r="D47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F47" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G47" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>89</v>
+      </c>
+      <c r="I47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="B50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C50" t="n">
         <v>2.3585</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H50" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>92</v>
+      </c>
+      <c r="I50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="B53" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C53" t="n">
         <v>2.571</v>
       </c>
       <c r="D53" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
@@ -1396,40 +1467,46 @@
         <v>15</v>
       </c>
       <c r="H53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>12</v>
+      </c>
+      <c r="I53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="B56" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" t="n">
         <v>2.7565</v>
       </c>
       <c r="D56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E56" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F56" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G56" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H56" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>98</v>
+      </c>
+      <c r="I56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="B57" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C57" t="n">
         <v>2.5</v>
@@ -1438,163 +1515,181 @@
         <v>15</v>
       </c>
       <c r="E57" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F57" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H57" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="B60" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C60" t="n">
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E60" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G60" t="s">
         <v>15</v>
       </c>
       <c r="H60" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>102</v>
+      </c>
+      <c r="I60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="B61" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C61" t="n">
         <v>1.546</v>
       </c>
       <c r="D61" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E61" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F61" t="s">
         <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H61" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>104</v>
+      </c>
+      <c r="I61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="B64" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C64" t="n">
         <v>2.714</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E64" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F64" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H64" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C67" t="n">
         <v>2.273</v>
       </c>
       <c r="D67" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" t="s">
         <v>18</v>
       </c>
-      <c r="E67" t="s">
-        <v>103</v>
-      </c>
-      <c r="F67" t="s">
-        <v>17</v>
-      </c>
       <c r="G67" t="s">
         <v>15</v>
       </c>
       <c r="H67" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>107</v>
+      </c>
+      <c r="I67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="B68" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C68" t="n">
         <v>2.636</v>
       </c>
       <c r="D68" t="s">
+        <v>108</v>
+      </c>
+      <c r="E68" t="s">
+        <v>104</v>
+      </c>
+      <c r="F68" t="s">
         <v>107</v>
       </c>
-      <c r="E68" t="s">
-        <v>103</v>
-      </c>
-      <c r="F68" t="s">
-        <v>106</v>
-      </c>
       <c r="G68" t="s">
         <v>15</v>
       </c>
       <c r="H68" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>109</v>
+      </c>
+      <c r="I68" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="B69" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C69" t="n">
         <v>2.909</v>
       </c>
       <c r="D69" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F69" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G69" t="s">
         <v>15</v>
@@ -1602,145 +1697,163 @@
       <c r="H69" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="I69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="B72" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C72" t="n">
         <v>2.678</v>
       </c>
       <c r="D72" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E72" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F72" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G72" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H72" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>115</v>
+      </c>
+      <c r="I72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="B75" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C75" t="n">
         <v>2</v>
       </c>
       <c r="D75" t="s">
+        <v>38</v>
+      </c>
+      <c r="E75" t="s">
+        <v>69</v>
+      </c>
+      <c r="F75" t="s">
+        <v>69</v>
+      </c>
+      <c r="G75" t="s">
+        <v>38</v>
+      </c>
+      <c r="H75" t="s">
         <v>37</v>
       </c>
-      <c r="E75" t="s">
-        <v>68</v>
-      </c>
-      <c r="F75" t="s">
-        <v>68</v>
-      </c>
-      <c r="G75" t="s">
-        <v>37</v>
-      </c>
-      <c r="H75" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="I75" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="B76" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C76" t="n">
         <v>2.6675</v>
       </c>
       <c r="D76" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E76" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F76" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G76" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H76" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+        <v>118</v>
+      </c>
+      <c r="I76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="B79" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C79" t="n">
         <v>2.333</v>
       </c>
       <c r="D79" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E79" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F79" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G79" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H79" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <v>34</v>
+      </c>
+      <c r="I79" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="B82" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C82" t="n">
         <v>2.176</v>
       </c>
       <c r="D82" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E82" t="s">
+        <v>122</v>
+      </c>
+      <c r="F82" t="s">
         <v>121</v>
       </c>
-      <c r="F82" t="s">
-        <v>120</v>
-      </c>
       <c r="G82" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H82" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+        <v>124</v>
+      </c>
+      <c r="I82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="B83" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C83" t="n">
         <v>1.938</v>
@@ -1749,174 +1862,195 @@
         <v>15</v>
       </c>
       <c r="E83" t="s">
+        <v>87</v>
+      </c>
+      <c r="F83" t="s">
         <v>86</v>
       </c>
-      <c r="F83" t="s">
-        <v>85</v>
-      </c>
       <c r="G83" t="s">
         <v>15</v>
       </c>
       <c r="H83" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>125</v>
+      </c>
+      <c r="I83" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="B86" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C86" t="n">
         <v>2.9885</v>
       </c>
       <c r="D86" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E86" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F86" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G86" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H86" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+        <v>76</v>
+      </c>
+      <c r="I86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="B89" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C89" t="n">
         <v>2.214</v>
       </c>
       <c r="D89" t="s">
+        <v>14</v>
+      </c>
+      <c r="E89" t="s">
         <v>13</v>
       </c>
-      <c r="E89" t="s">
-        <v>12</v>
-      </c>
       <c r="F89" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G89" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H89" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <v>13</v>
+      </c>
+      <c r="I89" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="B90" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C90" t="n">
         <v>1.546</v>
       </c>
       <c r="D90" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E90" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F90" t="s">
         <v>15</v>
       </c>
       <c r="G90" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H90" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>104</v>
+      </c>
+      <c r="I90" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="B93" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C93" t="n">
         <v>2.684</v>
       </c>
       <c r="D93" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E93" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F93" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G93" t="s">
+        <v>64</v>
+      </c>
+      <c r="H93" t="s">
         <v>63</v>
       </c>
-      <c r="H93" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="I93" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="B96" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C96" t="n">
         <v>2.933</v>
       </c>
       <c r="D96" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E96" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F96" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G96" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H96" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>135</v>
+      </c>
+      <c r="I96" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="B97" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C97" t="n">
         <v>2.79</v>
       </c>
       <c r="D97" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E97" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F97" t="s">
+        <v>64</v>
+      </c>
+      <c r="G97" t="s">
+        <v>62</v>
+      </c>
+      <c r="H97" t="s">
         <v>63</v>
       </c>
-      <c r="G97" t="s">
-        <v>61</v>
-      </c>
-      <c r="H97" t="s">
-        <v>62</v>
+      <c r="I97" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>